<commit_message>
add function for regular linear regression, updated interpretation words and accuracy
</commit_message>
<xml_diff>
--- a/output data/hazard_extraction_accuracy_v2.xlsx
+++ b/output data/hazard_extraction_accuracy_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srandrad\smart_nlp\output data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149A7685-41B5-4024-B4C5-F8DF6564A984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E95E255-517B-4B29-B23B-5A26D6AFBA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2412" yWindow="3660" windowWidth="17280" windowHeight="10044" firstSheet="15" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Command Transitions" sheetId="1" r:id="rId1"/>
@@ -731,51 +731,6 @@
     <t>2012_ID-FHA-012006_ROOSTER ROCK_2</t>
   </si>
   <si>
-    <t>2013_CA-KNF-005949_FORKS COMPLEX_96</t>
-  </si>
-  <si>
-    <t>2009_AK-CRS-914362_CHAKINA_29</t>
-  </si>
-  <si>
-    <t>2009_CA-BDF-13278_SHEEP_14</t>
-  </si>
-  <si>
-    <t>2010_AK-TAD-000128_TOKLAT_23</t>
-  </si>
-  <si>
-    <t>2008_VA-GDR-080002_SOUTH 1_7</t>
-  </si>
-  <si>
-    <t>2010_AK-TAD-000128_TOKLAT_19</t>
-  </si>
-  <si>
-    <t>2007_WA-OWF-000434_DOMKE LAKE COMPLEX_29</t>
-  </si>
-  <si>
-    <t>2007_MT-BDF-048_PATTENGAIL CREEK_33</t>
-  </si>
-  <si>
-    <t>2012_MT-FNF-000017_CONDON MOUNTAIN_35</t>
-  </si>
-  <si>
-    <t>2012_CO-PSF-556_SPRINGER_3</t>
-  </si>
-  <si>
-    <t>2009_CA-LNU-7027_PINE_2</t>
-  </si>
-  <si>
-    <t>2013_CA-TGU-6768_DEER_5</t>
-  </si>
-  <si>
-    <t>2006_MN-SUF-060249_TURTLE LAKE_18</t>
-  </si>
-  <si>
-    <t>2009_CA-SHU-5594_SHU LIGHTNING_21</t>
-  </si>
-  <si>
-    <t>2010_AK-TAD-000222_CHITANATALA_10</t>
-  </si>
-  <si>
     <t>2011_AZ-KNF-000631_BEALE_5</t>
   </si>
   <si>
@@ -885,6 +840,51 @@
   </si>
   <si>
     <t>Dry Weather</t>
+  </si>
+  <si>
+    <t>2010_AK-MSS-001278_EKLUTNA_0</t>
+  </si>
+  <si>
+    <t>2008_AZ-PPA-000056_SOLANO_0</t>
+  </si>
+  <si>
+    <t>2012_WA-OWF-000610_OKANOGAN COMPLEX_6</t>
+  </si>
+  <si>
+    <t>2013_CA-KNF-005949_FORKS COMPLEX_67</t>
+  </si>
+  <si>
+    <t>2013_MT-SWS-000068_LOLO CREEK COMPLEX_4</t>
+  </si>
+  <si>
+    <t>2011_AZ-CNF-011047_HORSESHOE 2_30</t>
+  </si>
+  <si>
+    <t>2012_WA-OWF-000610_OKANOGAN COMPLEX_5</t>
+  </si>
+  <si>
+    <t>2006_WY-SHF-000152_BOMBER BASIN_0</t>
+  </si>
+  <si>
+    <t>2013_MT-SWS-000068_LOLO CREEK COMPLEX_3</t>
+  </si>
+  <si>
+    <t>2006_CA-SHF-001693_BAR COMPLEX_110</t>
+  </si>
+  <si>
+    <t>2006_MT-GNF-055_PARADISE VALLEY COMPLEX_50</t>
+  </si>
+  <si>
+    <t>2013_ID-SCF-13165_LODGEPOLE_7</t>
+  </si>
+  <si>
+    <t>2006_WY-SHF-000152_BOMBER BASIN_1</t>
+  </si>
+  <si>
+    <t>2012_UT-NWS-000507_FLOOD CANYON_4</t>
+  </si>
+  <si>
+    <t>2013_CA-STF-002857_RIM_15</t>
   </si>
 </sst>
 </file>
@@ -2324,7 +2324,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection sqref="A1:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2339,7 +2339,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>227</v>
+        <v>264</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2347,7 +2347,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>228</v>
+        <v>265</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2355,7 +2355,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>229</v>
+        <v>266</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2363,7 +2363,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>230</v>
+        <v>267</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2371,47 +2371,47 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>231</v>
+        <v>268</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>232</v>
+        <v>269</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>233</v>
+        <v>270</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>234</v>
+        <v>271</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>235</v>
+        <v>272</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>236</v>
+        <v>273</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2419,7 +2419,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>237</v>
+        <v>274</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -2427,7 +2427,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>238</v>
+        <v>275</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2435,7 +2435,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>239</v>
+        <v>276</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -2443,7 +2443,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>240</v>
+        <v>277</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2451,16 +2451,16 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>241</v>
+        <v>278</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17">
-        <f xml:space="preserve"> SUM(B2:B16)</f>
-        <v>10</v>
+        <f>SUM(B2:B16)</f>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2496,7 +2496,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2504,7 +2504,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2512,7 +2512,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2520,7 +2520,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2528,7 +2528,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2536,7 +2536,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2544,7 +2544,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2552,7 +2552,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2560,7 +2560,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2568,7 +2568,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -2576,7 +2576,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2584,7 +2584,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2592,7 +2592,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2600,7 +2600,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2618,37 +2618,37 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="B2">
         <v>2882</v>
@@ -2669,7 +2669,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="B3">
         <v>861</v>
@@ -2690,7 +2690,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="B4">
         <v>3896</v>
@@ -2711,7 +2711,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="B5">
         <v>12802</v>
@@ -2732,7 +2732,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="B6">
         <v>196</v>
@@ -2753,7 +2753,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="B7">
         <v>728</v>
@@ -2774,7 +2774,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="B8">
         <v>3395</v>
@@ -2795,7 +2795,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="B9">
         <v>902</v>
@@ -2816,7 +2816,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="B10">
         <v>181</v>
@@ -2837,7 +2837,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="B11">
         <v>816</v>
@@ -2858,7 +2858,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="B12">
         <v>3343</v>
@@ -2879,7 +2879,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="B13">
         <v>535</v>
@@ -2900,7 +2900,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="B14">
         <v>2249</v>
@@ -2921,7 +2921,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="B15">
         <v>156</v>
@@ -2942,7 +2942,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="B16">
         <v>825</v>
@@ -2961,9 +2961,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="B17">
         <v>285</v>
@@ -2975,16 +2975,16 @@
         <v>5.2631578947368418E-2</v>
       </c>
       <c r="E17">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="B18">
         <v>2857</v>
@@ -3003,10 +3003,14 @@
         <v>0.93333333333333335</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F20">
         <f>AVERAGE(F2:F18)</f>
-        <v>0.94509803921568625</v>
+        <v>0.9529411764705884</v>
+      </c>
+      <c r="G20">
+        <f>_xlfn.STDEV.S(F2:F18)</f>
+        <v>6.1303914513190109E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>